<commit_message>
change api doc - add photo from post api
</commit_message>
<xml_diff>
--- a/docs/API명세서.xlsx
+++ b/docs/API명세서.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11955" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11955" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="목록" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="219">
   <si>
     <t>설명</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -638,12 +638,6 @@
   </si>
   <si>
     <t>{
-    "gram": "나는야 꿀벌개발자!"
-}</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
     "post_id": 37,
     "user_id": "honeybeeveloper"
 }</t>
@@ -905,12 +899,43 @@
     <t>언팔로우한 아이디</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>{
+    "gram": "나는야 꿀벌개발자!",
+    "photo_1": "D:\toy-output\youtoogram\20221017\honeybeeveloper\1.jpg",
+    "photo_2": "D:\toy-output\youtoogram\20221017\honeybeeveloper\2.jpg",
+    "photo_3": "D:\toy-output\youtoogram\20221017\honeybeeveloper\3.jpg",
+    "photo_4": "D:\toy-output\youtoogram\20221017\honeybeeveloper\4.jpg",
+    "photo_5": "D:\toy-output\youtoogram\20221017\honeybeeveloper\5.jpg"
+}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>multipart/form-data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 2</t>
+  </si>
+  <si>
+    <t>사진 3</t>
+  </si>
+  <si>
+    <t>사진 4</t>
+  </si>
+  <si>
+    <t>사진 5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -985,13 +1010,6 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="2" tint="-0.249977111117893"/>
-      <name val="돋움체"/>
-      <family val="3"/>
-      <charset val="129"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1118,7 +1136,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1183,24 +1201,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1213,26 +1213,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1253,6 +1237,40 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1262,19 +1280,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1562,7 +1568,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1651,7 +1657,7 @@
         <v>56</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>73</v>
@@ -1665,7 +1671,7 @@
         <v>57</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>74</v>
@@ -1679,7 +1685,7 @@
         <v>58</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>75</v>
@@ -1693,7 +1699,7 @@
         <v>59</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>76</v>
@@ -1707,7 +1713,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>77</v>
@@ -1735,7 +1741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1750,111 +1756,111 @@
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>207</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="35" t="s">
+      <c r="B1" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36" t="s">
-        <v>209</v>
-      </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>208</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="B2" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="30">
+      <c r="E4" s="35"/>
+      <c r="F4" s="33">
         <v>5000</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="35"/>
+      <c r="F5" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
+      <c r="B6" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="30" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
@@ -1903,40 +1909,40 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
@@ -1966,12 +1972,12 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>148</v>
@@ -1983,44 +1989,44 @@
         <v>40</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
     </row>
     <row r="16" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
+      <c r="A16" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -2029,14 +2035,14 @@
       <c r="B18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
@@ -2045,12 +2051,12 @@
       <c r="B19" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
@@ -2059,24 +2065,24 @@
       <c r="B20" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="28"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="22"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -2106,15 +2112,15 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>28</v>
@@ -2123,20 +2129,20 @@
         <v>28</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>28</v>
@@ -2145,35 +2151,55 @@
         <v>28</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39"/>
     </row>
     <row r="26" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="25"/>
+      <c r="A26" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A15:H15"/>
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="C18:H18"/>
@@ -2181,26 +2207,6 @@
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2225,111 +2231,111 @@
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="35" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="30">
+      <c r="E4" s="35"/>
+      <c r="F4" s="33">
         <v>5000</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="35"/>
+      <c r="F5" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="30" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -2512,40 +2518,40 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
     </row>
     <row r="17" spans="1:8" ht="115.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="22"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
@@ -2554,14 +2560,14 @@
       <c r="B19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="22"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
@@ -2570,12 +2576,12 @@
       <c r="B20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
@@ -2584,24 +2590,24 @@
       <c r="B21" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="28"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="22"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
@@ -2652,36 +2658,38 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39"/>
     </row>
     <row r="26" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="25"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
@@ -2694,13 +2702,11 @@
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2726,111 +2732,111 @@
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="35" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="30">
+      <c r="E4" s="35"/>
+      <c r="F4" s="33">
         <v>5000</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="35"/>
+      <c r="F5" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="30" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
@@ -2879,40 +2885,40 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
@@ -2951,38 +2957,38 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -2991,14 +2997,14 @@
       <c r="B18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
@@ -3029,16 +3035,16 @@
       <c r="H20" s="43"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="28"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="22"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
@@ -3089,36 +3095,38 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="22"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="39"/>
     </row>
     <row r="25" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="25"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
@@ -3134,13 +3142,11 @@
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3167,111 +3173,111 @@
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="35" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="30">
+      <c r="E4" s="35"/>
+      <c r="F4" s="33">
         <v>5000</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="35"/>
+      <c r="F5" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="30" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
@@ -3344,40 +3350,40 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
     </row>
     <row r="12" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
@@ -3386,14 +3392,14 @@
       <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="39"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
@@ -3402,12 +3408,12 @@
       <c r="B15" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
@@ -3416,34 +3422,34 @@
       <c r="B16" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="22"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
@@ -3494,39 +3500,36 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="22"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="39"/>
     </row>
     <row r="22" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="25"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
@@ -3539,11 +3542,14 @@
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="A18:H18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3555,8 +3561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3570,111 +3576,111 @@
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="35" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="30">
+      <c r="E4" s="35"/>
+      <c r="F4" s="33">
         <v>5000</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="33"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="G5" s="34"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="30" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
@@ -3723,40 +3729,40 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
@@ -3810,97 +3816,127 @@
       <c r="A15" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="48"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="48"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="48"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="48"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="48"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="22"/>
-    </row>
-    <row r="21" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="25"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39"/>
+    </row>
+    <row r="21" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="24"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="28"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="22"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
@@ -3909,14 +3945,14 @@
       <c r="B23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="22"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="39"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="17">
@@ -3925,12 +3961,12 @@
       <c r="B24" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
@@ -3939,24 +3975,24 @@
       <c r="B25" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="28"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="22"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
@@ -3986,15 +4022,15 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>28</v>
@@ -4003,20 +4039,20 @@
         <v>28</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>28</v>
@@ -4025,42 +4061,40 @@
         <v>28</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="22"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="39"/>
     </row>
     <row r="31" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="25"/>
+      <c r="A31" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
@@ -4076,14 +4110,17 @@
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="A26:H26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4106,111 +4143,111 @@
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="35" t="s">
+      <c r="B1" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="B2" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="30">
+      <c r="E4" s="35"/>
+      <c r="F4" s="33">
         <v>5000</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="35"/>
+      <c r="F5" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="33"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6" s="34"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
@@ -4259,40 +4296,40 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
@@ -4322,15 +4359,15 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>40</v>
@@ -4339,44 +4376,44 @@
         <v>40</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
     </row>
     <row r="16" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
+      <c r="A16" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -4385,14 +4422,14 @@
       <c r="B18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
@@ -4401,12 +4438,12 @@
       <c r="B19" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
@@ -4415,24 +4452,24 @@
       <c r="B20" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="28"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="22"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -4462,15 +4499,15 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>28</v>
@@ -4479,20 +4516,20 @@
         <v>28</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>28</v>
@@ -4501,35 +4538,55 @@
         <v>28</v>
       </c>
       <c r="H24" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39"/>
+    </row>
+    <row r="26" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="31" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
-    </row>
-    <row r="26" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="25"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A15:H15"/>
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="C18:H18"/>
@@ -4537,26 +4594,6 @@
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4582,111 +4619,111 @@
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="35" t="s">
+      <c r="B1" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>177</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="B2" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="30">
+      <c r="E4" s="35"/>
+      <c r="F4" s="33">
         <v>5000</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="35"/>
+      <c r="F5" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
+      <c r="C6" s="34"/>
+      <c r="D6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="33"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="G6" s="34"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
@@ -4735,40 +4772,40 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
@@ -4798,15 +4835,15 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>40</v>
@@ -4815,20 +4852,20 @@
         <v>40</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>181</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>40</v>
@@ -4837,44 +4874,44 @@
         <v>40</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
     </row>
     <row r="17" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
+      <c r="A17" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="22"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
@@ -4883,14 +4920,14 @@
       <c r="B19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="22"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
@@ -4899,12 +4936,12 @@
       <c r="B20" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
@@ -4913,24 +4950,24 @@
       <c r="B21" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="28"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="22"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
@@ -4960,15 +4997,15 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>28</v>
@@ -4977,20 +5014,20 @@
         <v>28</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>28</v>
@@ -4999,20 +5036,20 @@
         <v>28</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>28</v>
@@ -5021,35 +5058,55 @@
         <v>28</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="22"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="39"/>
     </row>
     <row r="28" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="25"/>
+      <c r="A28" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A16:H16"/>
     <mergeCell ref="A28:H28"/>
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="C19:H19"/>
@@ -5057,26 +5114,6 @@
     <mergeCell ref="C21:H21"/>
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5102,111 +5139,111 @@
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36" t="s">
-        <v>191</v>
-      </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>192</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="B2" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="30">
+      <c r="E4" s="35"/>
+      <c r="F4" s="33">
         <v>5000</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="35"/>
+      <c r="F5" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="35"/>
+      <c r="F6" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
@@ -5255,40 +5292,40 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
@@ -5327,38 +5364,38 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -5367,14 +5404,14 @@
       <c r="B18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
@@ -5383,12 +5420,12 @@
       <c r="B19" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
@@ -5397,24 +5434,24 @@
       <c r="B20" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="28"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="22"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -5444,15 +5481,15 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>28</v>
@@ -5461,20 +5498,20 @@
         <v>28</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>28</v>
@@ -5483,20 +5520,20 @@
         <v>28</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>28</v>
@@ -5505,35 +5542,55 @@
         <v>28</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="39"/>
     </row>
     <row r="27" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="25"/>
+      <c r="A27" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A15:H15"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="C18:H18"/>
@@ -5541,26 +5598,6 @@
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5588,111 +5625,111 @@
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36" t="s">
-        <v>196</v>
-      </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="B2" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="30">
+      <c r="E4" s="35"/>
+      <c r="F4" s="33">
         <v>5000</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="35"/>
+      <c r="F5" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
+      <c r="B6" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="30" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
@@ -5741,40 +5778,40 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
@@ -5804,12 +5841,12 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
       <c r="D14" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>148</v>
@@ -5821,44 +5858,44 @@
         <v>40</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
     </row>
     <row r="16" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
+      <c r="A16" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -5867,14 +5904,14 @@
       <c r="B18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
@@ -5883,12 +5920,12 @@
       <c r="B19" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
@@ -5897,24 +5934,24 @@
       <c r="B20" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="28"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="22"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
@@ -5944,15 +5981,15 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>28</v>
@@ -5961,20 +5998,20 @@
         <v>28</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>28</v>
@@ -5983,35 +6020,55 @@
         <v>28</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39"/>
     </row>
     <row r="26" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="25"/>
+      <c r="A26" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A15:H15"/>
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="C18:H18"/>
@@ -6019,26 +6076,6 @@
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>